<commit_message>
commit from main to lib
</commit_message>
<xml_diff>
--- a/sub/libfile3.xlsx
+++ b/sub/libfile3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunkuo/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunkuo/Desktop/test/main/sub/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -349,7 +349,13 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>123123</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>